<commit_message>
Site updated: 2022-02-08 17:10:49
</commit_message>
<xml_diff>
--- a/WisGate/WisGate.xlsx
+++ b/WisGate/WisGate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\blog\blog\source\WisGate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC3A135-D429-454A-8B3F-75B3D6F4BC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7BFF6F-BB80-408A-A8F4-7695A3D51EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -218,10 +218,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">	180mmx120mmx43</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Weight (kg)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -247,6 +243,10 @@
   </si>
   <si>
     <t>SF16A18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	180x120x43</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -829,13 +829,13 @@
         <v>40</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -898,7 +898,7 @@
         <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>33</v>
@@ -1141,22 +1141,22 @@
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="F21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="6">
         <v>3.15</v>
@@ -1194,7 +1194,7 @@
         <v>54</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Site updated: 2022-02-10 15:05:35
</commit_message>
<xml_diff>
--- a/WisGate/WisGate.xlsx
+++ b/WisGate/WisGate.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\blog\blog\source\WisGate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7BFF6F-BB80-408A-A8F4-7695A3D51EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D096AFD9-7B0B-408F-A7D4-F51A016D4116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="WisGate Edge " sheetId="1" r:id="rId1"/>
+    <sheet name="WisGate Developer " sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="75">
   <si>
     <t>model</t>
   </si>
@@ -247,6 +248,54 @@
   </si>
   <si>
     <t xml:space="preserve">	180x120x43</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WisGate Developer D4 / D4+ / D4P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WisGate Developer D0 / D0+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WisGate Developer D3 / D3+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WisGate Developer D4H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WisGate Developer Base</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAK7244 / RAK7244C / RAK7244P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAK7246 / RAK7246G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAK7243 / RAK7243C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAK7248</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAK7271 / RAK7371</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -336,11 +385,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -371,6 +417,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -653,556 +703,556 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="28.375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="25.375" style="8" customWidth="1"/>
-    <col min="9" max="9" width="19.75" style="8" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="8"/>
+    <col min="1" max="1" width="25" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="28.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="25.375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="19.75" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="4" t="s">
+      <c r="B16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="4" t="s">
+      <c r="B17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>3.15</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>1.3</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>0.3</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>0.3</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1211,4 +1261,72 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8459FC79-70A8-4F41-B5B7-E1EFD5F96F69}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>